<commit_message>
Finished so that trixr4kdz can do her part cus she keeps on asking me to finish even though it shouldn't be my job.
</commit_message>
<xml_diff>
--- a/test_files/sixteen_tests/4-genes_6-edges_artificial-data_Sigmoidal_estimation_fixb-0_fixP-0_graph.xlsx
+++ b/test_files/sixteen_tests/4-genes_6-edges_artificial-data_Sigmoidal_estimation_fixb-0_fixP-0_graph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="11490" yWindow="-225" windowWidth="8130" windowHeight="9360" tabRatio="644" firstSheet="7" activeTab="7"/>
+    <workbookView xWindow="11490" yWindow="-225" windowWidth="8130" windowHeight="9360" tabRatio="644" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>CIN5</t>
   </si>
@@ -597,7 +597,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -758,7 +758,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1412,7 +1412,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCellId="1" sqref="B41 A1"/>
+      <selection activeCell="D35" sqref="D34:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1523,9 +1523,7 @@
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" s="22" t="s">
-        <v>23</v>
-      </c>
+      <c r="B41" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -1676,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1923,7 +1921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>

</xml_diff>